<commit_message>
fix revisi guru mapel
</commit_message>
<xml_diff>
--- a/public/excel/template-guru.xlsx
+++ b/public/excel/template-guru.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Office\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2200194-624F-4973-AA7C-34AEFDFC55C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F282858-A36C-4DE3-83E2-6F8AE7A1B176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D576C546-DE07-4A3F-8E4C-4FE0C51ED16B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BB8EC23C-913C-423A-A975-EF6DBF0E2D76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,12 +34,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>username</t>
+    <r>
+      <t xml:space="preserve">SILAHKAN MASUKKAN
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>USERNAME GURU</t>
+    </r>
   </si>
   <si>
-    <t>nama_guru</t>
+    <r>
+      <t xml:space="preserve">SILAHKAN MASUKKAN
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NAMA GURU</t>
+    </r>
+  </si>
+  <si>
+    <t>namaguru</t>
+  </si>
+  <si>
+    <t>Nama Guru</t>
   </si>
 </sst>
 </file>
@@ -49,13 +86,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -70,7 +106,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -89,8 +125,8 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,20 +441,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D528DB-6225-41C0-ACE5-E7A5109B1B29}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9EC24D4-2F95-4EB9-81CE-F112F4F100E1}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1"/>
-    <col min="2" max="2" width="61.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,8 +462,15 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bug Fix Import Guru
</commit_message>
<xml_diff>
--- a/public/excel/template-guru.xlsx
+++ b/public/excel/template-guru.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ketuntasan\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F282858-A36C-4DE3-83E2-6F8AE7A1B176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B002EFDE-DEEA-49D8-A0AC-A82B1BAA41D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BB8EC23C-913C-423A-A975-EF6DBF0E2D76}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <r>
       <t xml:space="preserve">SILAHKAN MASUKKAN
@@ -74,6 +74,23 @@
   </si>
   <si>
     <t>Nama Guru</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SILAHKAN MASUKKAN
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KODE GURU</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -123,10 +140,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,33 +462,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9EC24D4-2F95-4EB9-81CE-F112F4F100E1}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.77734375" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improved Feature guru import
</commit_message>
<xml_diff>
--- a/public/excel/template-guru.xlsx
+++ b/public/excel/template-guru.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ketuntasan\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B002EFDE-DEEA-49D8-A0AC-A82B1BAA41D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8220328E-AD1F-48C1-BB26-4E42EAFB4732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BB8EC23C-913C-423A-A975-EF6DBF0E2D76}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BB8EC23C-913C-423A-A975-EF6DBF0E2D76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <r>
       <t xml:space="preserve">SILAHKAN MASUKKAN
@@ -92,12 +89,40 @@
       <t>KODE GURU</t>
     </r>
   </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PETUNJUK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+SILAHKAN MASUKKAN KODE GURU
+DI ANTARA SYMBOL [ ]</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,8 +138,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +157,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -140,13 +179,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,42 +505,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9EC24D4-2F95-4EB9-81CE-F112F4F100E1}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.77734375" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.77734375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>